<commit_message>
BugFix del match de categorias Formas
</commit_message>
<xml_diff>
--- a/TorneoApp/TestTorneoApp/RegistroTest.xlsx
+++ b/TorneoApp/TestTorneoApp/RegistroTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camil\Documents\Zhang Fei\TorneoAdmin\TorneoApp\TestTorneoApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F70518-8DAF-4E07-80EE-DF7ABCC83553}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{225B296C-5CD1-4085-A537-98EB97569344}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1056,7 +1056,7 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1395,7 +1395,7 @@
         <v>18</v>
       </c>
       <c r="F8" s="1">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G8" s="1">
         <v>50</v>

</xml_diff>

<commit_message>
Added estrategoia MatchSanda y filtros principales
</commit_message>
<xml_diff>
--- a/TorneoApp/TestTorneoApp/RegistroTest.xlsx
+++ b/TorneoApp/TestTorneoApp/RegistroTest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camil\Documents\Zhang Fei\TorneoAdmin\TorneoApp\TestTorneoApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{225B296C-5CD1-4085-A537-98EB97569344}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E222C249-CFFD-4209-AA55-58071D50E1AD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RegistroTest3" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,17 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">RegistroTest3!$A$1:$N$25</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1056,7 +1066,7 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added metodos para vista de categorias formas y sanda
</commit_message>
<xml_diff>
--- a/TorneoApp/TestTorneoApp/RegistroTest.xlsx
+++ b/TorneoApp/TestTorneoApp/RegistroTest.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camil\Documents\Zhang Fei\TorneoAdmin\TorneoApp\TestTorneoApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92792B69-9DF2-4068-8444-978535E5A546}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AB50650-C823-43B8-9500-D02AC8FEE447}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="RegistroTest3" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">RegistroTest3!$A$1:$N$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">RegistroTest3!$A$1:$O$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="59">
   <si>
     <t>Marca temporal</t>
   </si>
@@ -98,9 +98,6 @@
     <t>correo default</t>
   </si>
   <si>
-    <t>Femme 1</t>
-  </si>
-  <si>
     <t>Femme 2</t>
   </si>
   <si>
@@ -123,6 +120,96 @@
   </si>
   <si>
     <t>0-1 año</t>
+  </si>
+  <si>
+    <t>Femme 5</t>
+  </si>
+  <si>
+    <t>Femme 6</t>
+  </si>
+  <si>
+    <t>6/23/2019 15:49:24</t>
+  </si>
+  <si>
+    <t>Femme 7</t>
+  </si>
+  <si>
+    <t>6/27/2019 15:49:24</t>
+  </si>
+  <si>
+    <t>Femme 8</t>
+  </si>
+  <si>
+    <t>Femme 9</t>
+  </si>
+  <si>
+    <t>Femme 10</t>
+  </si>
+  <si>
+    <t>6/23/2019 15:49:25</t>
+  </si>
+  <si>
+    <t>Femme 11</t>
+  </si>
+  <si>
+    <t>6/27/2019 15:49:25</t>
+  </si>
+  <si>
+    <t>Femme 12</t>
+  </si>
+  <si>
+    <t>Femme 13</t>
+  </si>
+  <si>
+    <t>Femme 14</t>
+  </si>
+  <si>
+    <t>6/23/2019 15:49:26</t>
+  </si>
+  <si>
+    <t>Femme 15</t>
+  </si>
+  <si>
+    <t>6/27/2019 15:49:26</t>
+  </si>
+  <si>
+    <t>Femme 16</t>
+  </si>
+  <si>
+    <t>Femme 17</t>
+  </si>
+  <si>
+    <t>Femme 18</t>
+  </si>
+  <si>
+    <t>Femme 19</t>
+  </si>
+  <si>
+    <t>Camila</t>
+  </si>
+  <si>
+    <t>Comfenalco</t>
+  </si>
+  <si>
+    <t>Sanda, Formas</t>
+  </si>
+  <si>
+    <t>Forma sin arma</t>
+  </si>
+  <si>
+    <t>Conny</t>
+  </si>
+  <si>
+    <t>Telefono Personal</t>
+  </si>
+  <si>
+    <t>Formas</t>
+  </si>
+  <si>
+    <t>Forma sin arma, Forma con arma</t>
+  </si>
+  <si>
+    <t>Forma con arma</t>
   </si>
 </sst>
 </file>
@@ -970,10 +1057,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -984,15 +1071,16 @@
     <col min="6" max="6" width="6.28515625" customWidth="1"/>
     <col min="7" max="7" width="6.140625" customWidth="1"/>
     <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.28515625" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.5703125" customWidth="1"/>
-    <col min="11" max="11" width="5.140625" customWidth="1"/>
-    <col min="12" max="12" width="4.28515625" customWidth="1"/>
-    <col min="13" max="13" width="12.140625" customWidth="1"/>
-    <col min="14" max="14" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1030,13 +1118,16 @@
         <v>11</v>
       </c>
       <c r="M1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -1044,7 +1135,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>14</v>
@@ -1056,28 +1147,34 @@
         <v>19</v>
       </c>
       <c r="G2" s="1">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>26</v>
+        <v>52</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="N2" s="1">
+      <c r="M2" s="1">
+        <v>3167527488</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O2" s="1">
         <v>3173694664</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -1085,7 +1182,7 @@
         <v>20</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>14</v>
@@ -1100,25 +1197,28 @@
         <v>60</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="N3" s="1">
+      <c r="M3" s="1">
+        <v>3167527488</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O3" s="1">
         <v>3173694664</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -1126,7 +1226,7 @@
         <v>20</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>14</v>
@@ -1141,25 +1241,28 @@
         <v>65</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="N4" s="1">
+      <c r="M4" s="1">
+        <v>3167527488</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O4" s="1">
         <v>3173694666</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
@@ -1167,7 +1270,7 @@
         <v>20</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>14</v>
@@ -1182,26 +1285,710 @@
         <v>70</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="M5" s="1">
+        <v>3167527488</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O5" s="1">
+        <v>3173694670</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="1">
+        <v>23</v>
+      </c>
+      <c r="G6" s="1">
+        <v>67</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="N5" s="1">
-        <v>3173694670</v>
+      <c r="L6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M6" s="1">
+        <v>3167527488</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O6" s="1">
+        <v>3173694671</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="1">
+        <v>24</v>
+      </c>
+      <c r="G7" s="1">
+        <v>68</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M7" s="1">
+        <v>3167527488</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O7" s="1">
+        <v>3173694673</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="1">
+        <v>25</v>
+      </c>
+      <c r="G8" s="1">
+        <v>50</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M8" s="1">
+        <v>3167527488</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O8" s="1">
+        <v>3173694675</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="1">
+        <v>26</v>
+      </c>
+      <c r="G9" s="1">
+        <v>69</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M9" s="1">
+        <v>3167527488</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O9" s="1">
+        <v>3173694677</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="1">
+        <v>27</v>
+      </c>
+      <c r="G10" s="1">
+        <v>80</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M10" s="1">
+        <v>3167527488</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O10" s="1">
+        <v>3173694679</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="1">
+        <v>28</v>
+      </c>
+      <c r="G11" s="1">
+        <v>70</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M11" s="1">
+        <v>3167527488</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O11" s="1">
+        <v>3173694681</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="1">
+        <v>29</v>
+      </c>
+      <c r="G12" s="1">
+        <v>61</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M12" s="1">
+        <v>3167527488</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O12" s="1">
+        <v>3173694683</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="1">
+        <v>30</v>
+      </c>
+      <c r="G13" s="1">
+        <v>71</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M13" s="1">
+        <v>3167527488</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O13" s="1">
+        <v>3173694685</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="1">
+        <v>31</v>
+      </c>
+      <c r="G14" s="1">
+        <v>30</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M14" s="1">
+        <v>3167527488</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O14" s="1">
+        <v>3173694687</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="1">
+        <v>32</v>
+      </c>
+      <c r="G15" s="1">
+        <v>72</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M15" s="1">
+        <v>3167527488</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O15" s="1">
+        <v>3173694689</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="1">
+        <v>33</v>
+      </c>
+      <c r="G16" s="1">
+        <v>85</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M16" s="1">
+        <v>3167527488</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O16" s="1">
+        <v>3173694691</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="1">
+        <v>34</v>
+      </c>
+      <c r="G17" s="1">
+        <v>73</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M17" s="1">
+        <v>3167527488</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O17" s="1">
+        <v>3173694693</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="1">
+        <v>35</v>
+      </c>
+      <c r="G18" s="1">
+        <v>40</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M18" s="1">
+        <v>3167527488</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O18" s="1">
+        <v>3173694695</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="1">
+        <v>36</v>
+      </c>
+      <c r="G19" s="1">
+        <v>74</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M19" s="1">
+        <v>3167527488</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O19" s="1">
+        <v>3173694697</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="1">
+        <v>37</v>
+      </c>
+      <c r="G20" s="1">
+        <v>44</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M20" s="1">
+        <v>3167527488</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O20" s="1">
+        <v>3173694699</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>